<commit_message>
Data update using gitrun.py
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>35</x:v>
@@ -719,16 +719,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>31</x:v>
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>10</x:v>
@@ -797,7 +797,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
         <x:v>5</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>23</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>21</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1083,16 +1083,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>32</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>33</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>34</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>31</x:v>
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>20</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>39</x:v>
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>16</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>58</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>17</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>24</x:v>
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>32</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>64</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>15</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>55</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>26</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>43</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>32</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>33</x:v>
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>3</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-06 19:56:30
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -670,13 +670,13 @@
         <x:v>61</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>13</x:v>
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>35</x:v>
@@ -878,13 +878,13 @@
         <x:v>201</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>214</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>110</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>18</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>34</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>26</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>25</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>52</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>48</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>60</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>32</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>30</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>54</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>61</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>84</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>34</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-07 06:00:41
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>10</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>76</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>28</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>24</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>41</x:v>
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1135,16 +1135,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>36</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>35</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>34</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>26</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>48</x:v>
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>19</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>49</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>60</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>53</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>32</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>24</x:v>
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1658,13 +1658,13 @@
         <x:v>139</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>71</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>17</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>65</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>31</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>56</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>200</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>30</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>51</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>34</x:v>
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,16 +1967,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-07 12:00:39
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>10</x:v>
@@ -823,16 +823,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E8" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="F8" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="G8" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H8" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>76</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>35</x:v>
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>28</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>26</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>69</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>52</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>48</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>53</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>40</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>56</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>17</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>65</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>31</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>56</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>204</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>85</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>30</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-07 18:00:42
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -849,16 +849,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E9" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="F9" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="G9" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H9" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>224</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>113</x:v>
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>28</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>19</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>35</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>49</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>34</x:v>
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>25</x:v>
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>49</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>61</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>53</x:v>
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>40</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>56</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>72</x:v>
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>56</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>85</x:v>
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>4</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-08 06:00:51
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -797,7 +797,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
         <x:v>7</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>207</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>77</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>226</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>13</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>73</x:v>
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>52</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>49</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>53</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>34</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>17</x:v>
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>64</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>31</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>56</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>214</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>31</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>51</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-08 12:00:41
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>37</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>77</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>115</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>24</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>42</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>20</x:v>
@@ -1164,13 +1164,13 @@
         <x:v>73</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1268,13 +1268,13 @@
         <x:v>103</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>28</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>73</x:v>
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>63</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1580,13 +1580,13 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>19</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>216</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>51</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-08 18:00:41
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>37</x:v>
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>38</x:v>
@@ -797,16 +797,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G7" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>210</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>77</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>28</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>24</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>19</x:v>
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>13</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>20</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>38</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>46</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>51</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>56</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,16 +1421,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>63</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>56</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>19</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>67</x:v>
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>218</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>88</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>33</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>51</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>35</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>38</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-09 06:00:43
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>232</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>35</x:v>
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>24</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1060,13 +1060,13 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1086,13 +1086,13 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1135,16 +1135,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>38</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>38</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>46</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>56</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>27</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>41</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>32</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>33</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1967,16 +1967,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-09 12:00:49
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -670,13 +670,13 @@
         <x:v>67</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -722,13 +722,13 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>10</x:v>
@@ -797,16 +797,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="G7" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>218</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -956,13 +956,13 @@
         <x:v>78</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -982,13 +982,13 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1083,16 +1083,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1112,13 +1112,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F19" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="G19" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H19" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:8">
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>21</x:v>
@@ -1164,13 +1164,13 @@
         <x:v>78</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>96</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1398,13 +1398,13 @@
         <x:v>116</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1424,13 +1424,13 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1502,13 +1502,13 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1554,13 +1554,13 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1632,13 +1632,13 @@
         <x:v>116</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>176</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1788,13 +1788,13 @@
         <x:v>65</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>5</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-09 18:02:05
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>45</x:v>
@@ -849,7 +849,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E9" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F9" s="0" t="n">
         <x:v>4</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>127</x:v>
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>52</x:v>
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>16</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>21</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>42</x:v>
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>51</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>60</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>47</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>34</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>74</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>39</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>5</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-09 22:51:53
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -693,7 +693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>20</x:v>
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>45</x:v>
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>10</x:v>
@@ -797,16 +797,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G7" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
@@ -852,13 +852,13 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="F9" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G9" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H9" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>94</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>252</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>23</x:v>
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>16</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>21</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>55</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>21</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>64</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>34</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>240</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>57</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>45</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>46</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-09 23:00:40
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>49</x:v>
@@ -1216,13 +1216,13 @@
         <x:v>112</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-10 06:00:42
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -719,16 +719,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>10</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>132</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>23</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1684,13 +1684,13 @@
         <x:v>215</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>79</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>250</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>110</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>41</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-10 12:00:41
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -670,13 +670,13 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -693,16 +693,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -719,16 +719,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -748,13 +748,13 @@
         <x:v>81</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -774,13 +774,13 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -800,13 +800,13 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="G7" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
@@ -826,13 +826,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="F8" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="G8" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H8" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>268</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1008,13 +1008,13 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1086,13 +1086,13 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1112,13 +1112,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="F19" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G19" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H19" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:8">
@@ -1138,13 +1138,13 @@
         <x:v>61</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1190,13 +1190,13 @@
         <x:v>106</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>112</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1294,13 +1294,13 @@
         <x:v>76</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1372,13 +1372,13 @@
         <x:v>113</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,16 +1421,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1476,13 +1476,13 @@
         <x:v>163</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1502,13 +1502,13 @@
         <x:v>124</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1788,13 +1788,13 @@
         <x:v>69</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1814,13 +1814,13 @@
         <x:v>152</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>251</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>5</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-10 23:00:41
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>261</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>118</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>279</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>39</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>40</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>70</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>25</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>51</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>68</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>52</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>102</x:v>
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>79</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>67</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>95</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>85</x:v>
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>108</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>264</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>141</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>55</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>55</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>59</x:v>
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>5</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-11 06:00:44
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>135</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>118</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>283</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>170</x:v>
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>39</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>40</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>62</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>79</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>218</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>119</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>105</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>55</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-11 12:00:45
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -670,13 +670,13 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -774,13 +774,13 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>270</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>284</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -956,13 +956,13 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -982,13 +982,13 @@
         <x:v>81</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1008,13 +1008,13 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>70</x:v>
@@ -1060,13 +1060,13 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>63</x:v>
@@ -1242,13 +1242,13 @@
         <x:v>131</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>113</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1372,13 +1372,13 @@
         <x:v>117</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1424,13 +1424,13 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1450,13 +1450,13 @@
         <x:v>120</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>86</x:v>
@@ -1528,13 +1528,13 @@
         <x:v>93</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>25</x:v>
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1606,13 +1606,13 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>231</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>119</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>35</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>5</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-11 18:00:43
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>57</x:v>
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>18</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>272</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>123</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>292</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>178</x:v>
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>41</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>30</x:v>
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>20</x:v>
@@ -1135,16 +1135,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>63</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>72</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>52</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>74</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>26</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>176</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>93</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>25</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>55</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>46</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>84</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>232</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>113</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>42</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>109</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>276</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>146</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>56</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>61</x:v>
@@ -1967,16 +1967,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-11 23:00:45
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>18</x:v>
@@ -797,7 +797,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
         <x:v>16</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>283</x:v>
+        <x:v>298</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>200</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>294</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -956,13 +956,13 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>41</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>30</x:v>
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>20</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>106</x:v>
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>74</x:v>
@@ -1398,13 +1398,13 @@
         <x:v>138</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>55</x:v>
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>66</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>84</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>238</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>113</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>224</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>280</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>56</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>56</x:v>
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-12 06:59:58
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>18</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>80</x:v>
@@ -1684,13 +1684,13 @@
         <x:v>246</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1762,13 +1762,13 @@
         <x:v>194</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>43</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>111</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>288</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>148</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>56</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>81</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-12 12:13:10
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>20</x:v>
@@ -771,16 +771,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>298</x:v>
+        <x:v>302</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>209</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>306</x:v>
+        <x:v>311</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>41</x:v>
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1242,13 +1242,13 @@
         <x:v>137</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1294,13 +1294,13 @@
         <x:v>82</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>106</x:v>
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>45</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>74</x:v>
@@ -1398,13 +1398,13 @@
         <x:v>139</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>26</x:v>
@@ -1450,13 +1450,13 @@
         <x:v>126</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1554,13 +1554,13 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>48</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>66</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>176</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>84</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1736,13 +1736,13 @@
         <x:v>69</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>289</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-12 18:00:50
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -693,16 +693,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>20</x:v>
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>20</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>302</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>210</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>126</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>311</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>185</x:v>
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>49</x:v>
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>41</x:v>
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>20</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>55</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>65</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>73</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>77</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>55</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>200</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>45</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>74</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>82</x:v>
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>26</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>71</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>102</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>92</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>60</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>57</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>66</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>84</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>247</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>230</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>125</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>39</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>110</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>44</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>291</x:v>
+        <x:v>297</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>56</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>86</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>59</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>64</x:v>
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>6</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-12 23:00:42
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -693,7 +693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>24</x:v>
@@ -719,16 +719,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -823,7 +823,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E8" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="F8" s="0" t="n">
         <x:v>3</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>306</x:v>
+        <x:v>319</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>126</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>315</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>185</x:v>
@@ -982,13 +982,13 @@
         <x:v>88</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>74</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>31</x:v>
@@ -1109,7 +1109,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E19" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="F19" s="0" t="n">
         <x:v>5</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>55</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>65</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>73</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>55</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>71</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>102</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>92</x:v>
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>57</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>48</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>66</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>253</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>39</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>44</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>199</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>297</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>56</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>86</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>155</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>59</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>64</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-13 07:15:58
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>319</x:v>
+        <x:v>321</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>153</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>218</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>126</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>322</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>185</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>74</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>31</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>65</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>73</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>55</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>204</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>102</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>61</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>66</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>119</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>243</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>127</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>207</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>114</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>153</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>56</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-13 12:00:44
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -719,16 +719,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -774,13 +774,13 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>321</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>325</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1008,13 +1008,13 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>31</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1294,13 +1294,13 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>46</x:v>
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>205</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>99</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>57</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>48</x:v>
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>264</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>216</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>44</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>305</x:v>
+        <x:v>308</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1866,13 +1866,13 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>64</x:v>
@@ -1970,13 +1970,13 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-13 18:00:46
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>56</x:v>
@@ -693,7 +693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>24</x:v>
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>62</x:v>
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>22</x:v>
@@ -797,7 +797,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
         <x:v>16</x:v>
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>329</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>158</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>127</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>327</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>44</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>20</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>74</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>81</x:v>
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>217</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>114</x:v>
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>26</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>94</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>62</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>30</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>57</x:v>
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>273</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>123</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>41</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>114</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>44</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>308</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>155</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>155</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>59</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>63</x:v>
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,16 +1967,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-13 23:00:46
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>56</x:v>
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>22</x:v>
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>62</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>334</x:v>
+        <x:v>342</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>334</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>190</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>46</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>31</x:v>
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>20</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>58</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>68</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>47</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>78</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>26</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>73</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>216</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>62</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>30</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>57</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>49</x:v>
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>284</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>41</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>230</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>44</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>218</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>318</x:v>
+        <x:v>323</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>156</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>59</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>63</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>65</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-14 07:15:43
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>22</x:v>
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>342</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>159</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>237</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>128</x:v>
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>53</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>155</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>68</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>59</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>237</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>115</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>87</x:v>
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>26</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>95</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>69</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>136</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>239</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>115</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>323</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>156</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-14 12:00:46
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>56</x:v>
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>62</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>344</x:v>
+        <x:v>348</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>238</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>128</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>343</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>75</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>82</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>59</x:v>
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>26</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>73</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>108</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>62</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>69</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>290</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>126</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>136</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>41</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>240</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>115</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>325</x:v>
+        <x:v>326</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>156</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>59</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>210</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1918,13 +1918,13 @@
         <x:v>185</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-14 18:00:46
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>348</x:v>
+        <x:v>349</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>160</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>344</x:v>
+        <x:v>347</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>46</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>68</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>238</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>115</x:v>
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>47</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>78</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>108</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>95</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>62</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>291</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>126</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>258</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1788,13 +1788,13 @@
         <x:v>99</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>226</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>326</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>59</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>91</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-14 23:00:43
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>349</x:v>
+        <x:v>353</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>160</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>240</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>128</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>347</x:v>
+        <x:v>350</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>53</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>31</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>68</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>78</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>108</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>49</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>293</x:v>
+        <x:v>297</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>262</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>137</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>41</x:v>
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>121</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>329</x:v>
+        <x:v>332</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>157</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>59</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>218</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>91</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-15 07:16:02
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>353</x:v>
+        <x:v>355</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>160</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>84</x:v>
@@ -1528,13 +1528,13 @@
         <x:v>107</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>121</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>332</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>157</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>59</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-15 12:00:50
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>63</x:v>
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>355</x:v>
+        <x:v>357</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>160</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>350</x:v>
+        <x:v>351</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>193</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>46</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>77</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>239</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>115</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>297</x:v>
+        <x:v>299</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>127</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>243</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>115</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>44</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>230</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>121</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>69</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-15 18:00:48
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>57</x:v>
@@ -693,16 +693,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>357</x:v>
+        <x:v>364</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>241</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>128</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>351</x:v>
+        <x:v>356</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>44</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>77</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>31</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>77</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>60</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>241</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>47</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>30</x:v>
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>204</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>299</x:v>
+        <x:v>300</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>127</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>264</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>139</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>115</x:v>
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>231</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>333</x:v>
+        <x:v>339</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>59</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-15 23:00:46
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>64</x:v>
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>22</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>364</x:v>
+        <x:v>369</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>166</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>128</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>356</x:v>
+        <x:v>362</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>46</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>77</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>31</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>59</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>26</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>96</x:v>
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>300</x:v>
+        <x:v>302</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>267</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>339</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>158</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>59</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>68</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>70</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-16 07:16:06
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>369</x:v>
+        <x:v>370</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>166</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>207</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>85</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>115</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>343</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-16 12:00:42
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -722,13 +722,13 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -774,13 +774,13 @@
         <x:v>37</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>370</x:v>
+        <x:v>372</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>362</x:v>
+        <x:v>363</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>203</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -956,13 +956,13 @@
         <x:v>102</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>60</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1294,13 +1294,13 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>248</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1372,13 +1372,13 @@
         <x:v>138</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1398,13 +1398,13 @@
         <x:v>163</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1424,13 +1424,13 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1476,13 +1476,13 @@
         <x:v>230</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1502,13 +1502,13 @@
         <x:v>166</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>49</x:v>
@@ -1632,13 +1632,13 @@
         <x:v>152</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1658,13 +1658,13 @@
         <x:v>208</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>302</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>247</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>234</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>344</x:v>
+        <x:v>345</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>155</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>224</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1944,13 +1944,13 @@
         <x:v>186</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,16 +1967,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-16 18:00:51
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -748,13 +748,13 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -797,7 +797,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
         <x:v>16</x:v>
@@ -849,7 +849,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E9" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F9" s="0" t="n">
         <x:v>5</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>372</x:v>
+        <x:v>380</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>248</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>363</x:v>
+        <x:v>366</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>203</x:v>
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>48</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>79</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>31</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>60</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>83</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>49</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>78</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>91</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>82</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>230</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>58</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>72</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>87</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>304</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>270</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>145</x:v>
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>48</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>236</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>345</x:v>
+        <x:v>349</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>163</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>63</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>95</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>75</x:v>
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>10</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-16 23:00:40
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>23</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>380</x:v>
+        <x:v>388</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>134</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>366</x:v>
+        <x:v>369</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>48</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>79</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>31</x:v>
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>20</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>60</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>69</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>72</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>83</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>88</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>253</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>121</x:v>
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>49</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>113</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>70</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>30</x:v>
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>49</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>72</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>210</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>306</x:v>
+        <x:v>313</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>272</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>45</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>116</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>238</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>349</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>232</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>95</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-17 07:00:45
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>60</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>66</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>235</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>113</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>30</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>49</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>72</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>279</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>146</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>64</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-17 12:00:46
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -722,13 +722,13 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -774,13 +774,13 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>388</x:v>
+        <x:v>390</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -904,13 +904,13 @@
         <x:v>258</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>369</x:v>
+        <x:v>375</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>204</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>204</x:v>
+        <x:v>208</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1034,13 +1034,13 @@
         <x:v>164</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1164,13 +1164,13 @@
         <x:v>122</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1190,13 +1190,13 @@
         <x:v>143</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1242,13 +1242,13 @@
         <x:v>165</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>151</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1424,13 +1424,13 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1450,13 +1450,13 @@
         <x:v>154</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>236</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1502,13 +1502,13 @@
         <x:v>170</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>112</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1554,13 +1554,13 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1606,13 +1606,13 @@
         <x:v>79</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1684,13 +1684,13 @@
         <x:v>313</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1710,13 +1710,13 @@
         <x:v>281</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1762,13 +1762,13 @@
         <x:v>250</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1788,13 +1788,13 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1814,13 +1814,13 @@
         <x:v>244</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1840,13 +1840,13 @@
         <x:v>352</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1970,13 +1970,13 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-17 18:00:56
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>58</x:v>
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>25</x:v>
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>73</x:v>
@@ -771,16 +771,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>390</x:v>
+        <x:v>393</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>258</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>375</x:v>
+        <x:v>378</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>211</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>54</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>81</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>35</x:v>
@@ -1083,16 +1083,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>65</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>71</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>73</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>257</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>93</x:v>
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>29</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>237</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>121</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>72</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>61</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>75</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>214</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>95</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>313</x:v>
+        <x:v>316</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>281</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>151</x:v>
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>250</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>119</x:v>
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>136</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>352</x:v>
+        <x:v>355</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>66</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>236</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1918,13 +1918,13 @@
         <x:v>207</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>79</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-17 23:00:45
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>58</x:v>
@@ -722,13 +722,13 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>393</x:v>
+        <x:v>398</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>260</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>378</x:v>
+        <x:v>386</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>211</x:v>
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>49</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>49</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>35</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>71</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>69</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>261</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>240</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>121</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>72</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>31</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>316</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>286</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>49</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>252</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>355</x:v>
+        <x:v>362</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>241</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>102</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>207</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>84</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>79</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-18 07:00:43
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>58</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>398</x:v>
+        <x:v>400</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>386</x:v>
+        <x:v>387</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>211</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>73</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>103</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>289</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>152</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>67</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-18 12:00:42
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -670,13 +670,13 @@
         <x:v>87</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -696,13 +696,13 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -748,13 +748,13 @@
         <x:v>119</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>400</x:v>
+        <x:v>403</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>272</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>387</x:v>
+        <x:v>388</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>214</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -982,13 +982,13 @@
         <x:v>99</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1060,13 +1060,13 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>26</x:v>
@@ -1164,13 +1164,13 @@
         <x:v>124</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1190,13 +1190,13 @@
         <x:v>145</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>169</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>200</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1320,13 +1320,13 @@
         <x:v>263</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1450,13 +1450,13 @@
         <x:v>159</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>242</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>31</x:v>
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1606,13 +1606,13 @@
         <x:v>79</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1658,13 +1658,13 @@
         <x:v>217</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1684,13 +1684,13 @@
         <x:v>322</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>290</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1762,13 +1762,13 @@
         <x:v>255</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1788,13 +1788,13 @@
         <x:v>113</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>252</x:v>
+        <x:v>254</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>137</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>362</x:v>
+        <x:v>365</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1866,13 +1866,13 @@
         <x:v>171</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>243</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-18 18:00:53
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>59</x:v>
@@ -693,7 +693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>26</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>403</x:v>
+        <x:v>404</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>273</x:v>
+        <x:v>275</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>147</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>388</x:v>
+        <x:v>391</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>214</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>214</x:v>
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>56</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>51</x:v>
@@ -1138,13 +1138,13 @@
         <x:v>77</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>74</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>92</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>93</x:v>
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>263</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>127</x:v>
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>53</x:v>
@@ -1398,13 +1398,13 @@
         <x:v>172</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>123</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>62</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>52</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>76</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>217</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>322</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>149</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>292</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>156</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>121</x:v>
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>254</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>137</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>365</x:v>
+        <x:v>366</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>179</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>68</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>103</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>209</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>79</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-18 23:00:48
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -693,7 +693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>26</x:v>
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>26</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>404</x:v>
+        <x:v>408</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>202</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>275</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>391</x:v>
+        <x:v>401</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>217</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>50</x:v>
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>36</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>205</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>265</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>127</x:v>
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>79</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>97</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>93</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>247</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>123</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>107</x:v>
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>62</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>52</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>76</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>99</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>324</x:v>
+        <x:v>326</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>149</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>293</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>50</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>56</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>256</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>366</x:v>
+        <x:v>370</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>68</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>199</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>79</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-19 07:00:47
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>408</x:v>
+        <x:v>409</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>202</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>276</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>146</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>222</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>326</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>149</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>296</x:v>
+        <x:v>297</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>158</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-19 12:00:51
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -670,13 +670,13 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -748,13 +748,13 @@
         <x:v>120</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -774,13 +774,13 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>409</x:v>
+        <x:v>413</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>206</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -904,13 +904,13 @@
         <x:v>277</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>401</x:v>
+        <x:v>402</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>217</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>217</x:v>
+        <x:v>220</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>56</x:v>
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1086,13 +1086,13 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1138,13 +1138,13 @@
         <x:v>77</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1190,13 +1190,13 @@
         <x:v>145</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>75</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>209</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>268</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1372,13 +1372,13 @@
         <x:v>143</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1398,13 +1398,13 @@
         <x:v>174</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,16 +1421,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1476,13 +1476,13 @@
         <x:v>248</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1502,13 +1502,13 @@
         <x:v>178</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>117</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>32</x:v>
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>52</x:v>
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1658,13 +1658,13 @@
         <x:v>223</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1684,13 +1684,13 @@
         <x:v>327</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>297</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1788,13 +1788,13 @@
         <x:v>116</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>261</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>370</x:v>
+        <x:v>372</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1866,13 +1866,13 @@
         <x:v>175</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>248</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>103</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>200</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-19 18:00:57
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -693,7 +693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>26</x:v>
@@ -797,7 +797,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
         <x:v>16</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>413</x:v>
+        <x:v>414</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>207</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>277</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>402</x:v>
+        <x:v>405</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>220</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>220</x:v>
+        <x:v>221</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>56</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>53</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>28</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>68</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>176</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>99</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>75</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>273</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>54</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>248</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>125</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>110</x:v>
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>327</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>301</x:v>
+        <x:v>303</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>160</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>50</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>257</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1814,13 +1814,13 @@
         <x:v>263</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>372</x:v>
+        <x:v>375</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>184</x:v>
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>251</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>103</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>216</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-19 23:00:42
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>414</x:v>
+        <x:v>419</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>207</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>207</x:v>
+        <x:v>209</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>279</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>405</x:v>
+        <x:v>408</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>221</x:v>
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>56</x:v>
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>50</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>53</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>37</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>74</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>76</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>95</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>214</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>75</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>278</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>131</x:v>
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>54</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>80</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>77</x:v>
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>333</x:v>
+        <x:v>336</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>303</x:v>
+        <x:v>307</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>160</x:v>
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>127</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>58</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>263</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>375</x:v>
+        <x:v>377</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>184</x:v>
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>176</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>252</x:v>
+        <x:v>254</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1967,16 +1967,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-20 07:00:48
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>408</x:v>
+        <x:v>409</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>222</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>89</x:v>
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>28</x:v>
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1736,13 +1736,13 @@
         <x:v>103</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>72</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>80</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-20 12:00:49
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -774,13 +774,13 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>419</x:v>
+        <x:v>423</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>209</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>209</x:v>
+        <x:v>211</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>281</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>409</x:v>
+        <x:v>410</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>222</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>222</x:v>
+        <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -982,13 +982,13 @@
         <x:v>104</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1008,13 +1008,13 @@
         <x:v>136</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1034,13 +1034,13 @@
         <x:v>173</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1060,13 +1060,13 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1083,16 +1083,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>175</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>95</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1294,13 +1294,13 @@
         <x:v>124</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>279</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>167</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1450,13 +1450,13 @@
         <x:v>163</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1476,13 +1476,13 @@
         <x:v>249</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1502,13 +1502,13 @@
         <x:v>181</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>77</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>77</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>225</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1710,13 +1710,13 @@
         <x:v>307</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1736,13 +1736,13 @@
         <x:v>103</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>260</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>58</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>266</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1840,13 +1840,13 @@
         <x:v>377</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>254</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>217</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-20 18:00:55
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>285</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>410</x:v>
+        <x:v>414</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>223</x:v>
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>56</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>68</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>220</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>281</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>80</x:v>
@@ -1421,16 +1421,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>128</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>113</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>77</x:v>
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>63</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>52</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>226</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>336</x:v>
+        <x:v>337</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>157</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>268</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>147</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>377</x:v>
+        <x:v>381</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>188</x:v>
@@ -1866,13 +1866,13 @@
         <x:v>181</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>107</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>218</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-20 23:00:39
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>26</x:v>
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>287</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>414</x:v>
+        <x:v>417</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>224</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>56</x:v>
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>41</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>74</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>95</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>103</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>284</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>135</x:v>
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>250</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>128</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>77</x:v>
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>337</x:v>
+        <x:v>338</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>157</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>309</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>270</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>381</x:v>
+        <x:v>385</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>188</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>107</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>220</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>96</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>85</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-21 07:00:47
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>90</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>77</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>77</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>312</x:v>
+        <x:v>314</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>166</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>266</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>128</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-21 12:00:45
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>423</x:v>
+        <x:v>424</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>211</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>417</x:v>
+        <x:v>421</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>224</x:v>
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>56</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>55</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>90</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>224</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>103</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>80</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>98</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>252</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>128</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>114</x:v>
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>230</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>106</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>338</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>162</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>314</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>166</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>267</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>128</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>385</x:v>
+        <x:v>386</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-21 18:00:49
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>424</x:v>
+        <x:v>426</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>211</x:v>
@@ -904,13 +904,13 @@
         <x:v>291</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>421</x:v>
+        <x:v>424</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>224</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>224</x:v>
+        <x:v>227</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>56</x:v>
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>90</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>41</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>74</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>225</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>103</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>77</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>286</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>80</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>253</x:v>
+        <x:v>254</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>128</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>77</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>63</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>343</x:v>
+        <x:v>346</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>162</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>315</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>61</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>272</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>386</x:v>
+        <x:v>387</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>189</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>96</x:v>
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>209</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-21 23:00:44
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>426</x:v>
+        <x:v>431</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>213</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>291</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>162</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>424</x:v>
+        <x:v>426</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>227</x:v>
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>176</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>90</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>77</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>77</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>290</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>138</x:v>
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1421,16 +1421,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>254</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>128</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1580,13 +1580,13 @@
         <x:v>135</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>346</x:v>
+        <x:v>348</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>162</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>318</x:v>
+        <x:v>319</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>54</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>272</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>131</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>61</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>274</x:v>
+        <x:v>275</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>149</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>387</x:v>
+        <x:v>389</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>73</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>96</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-22 07:00:57
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>55</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>128</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>116</x:v>
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>77</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>64</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>348</x:v>
+        <x:v>349</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>162</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>54</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>225</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>96</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-22 12:00:47
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>431</x:v>
+        <x:v>433</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>213</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>292</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>162</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>426</x:v>
+        <x:v>427</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>54</x:v>
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>41</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>176</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>103</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>77</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>296</x:v>
+        <x:v>299</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>138</x:v>
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>98</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>128</x:v>
@@ -1502,13 +1502,13 @@
         <x:v>191</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>77</x:v>
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>232</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>106</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>349</x:v>
+        <x:v>351</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>162</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>319</x:v>
+        <x:v>320</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>168</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>273</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>131</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>61</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>275</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>149</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>258</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>108</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-22 18:00:51
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -797,7 +797,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
         <x:v>16</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>433</x:v>
+        <x:v>437</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>293</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>427</x:v>
+        <x:v>430</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>90</x:v>
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>74</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>78</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>230</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>103</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>77</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>299</x:v>
+        <x:v>298</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>138</x:v>
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>80</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>65</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>351</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>162</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>320</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>168</x:v>
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>274</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>389</x:v>
+        <x:v>390</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>191</x:v>
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>259</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>226</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>86</x:v>
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>10</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-22 23:00:46
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>61</x:v>
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>82</x:v>
@@ -797,7 +797,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
         <x:v>16</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>437</x:v>
+        <x:v>439</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>295</x:v>
+        <x:v>300</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>430</x:v>
+        <x:v>435</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>229</x:v>
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>54</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>42</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>69</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>74</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>78</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>96</x:v>
@@ -1268,13 +1268,13 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>62</x:v>
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>108</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>98</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>257</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>80</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>38</x:v>
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>106</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>352</x:v>
+        <x:v>356</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>322</x:v>
+        <x:v>326</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>278</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>390</x:v>
+        <x:v>394</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>191</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>262</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>109</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>10</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-23 07:00:53
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>62</x:v>
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>278</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>132</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>62</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>280</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-23 12:00:48
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -748,13 +748,13 @@
         <x:v>123</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -771,16 +771,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>439</x:v>
+        <x:v>442</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>216</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>216</x:v>
+        <x:v>217</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>300</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>168</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -930,13 +930,13 @@
         <x:v>435</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>233</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -956,13 +956,13 @@
         <x:v>114</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1008,13 +1008,13 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1086,13 +1086,13 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1190,13 +1190,13 @@
         <x:v>151</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1268,13 +1268,13 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>298</x:v>
+        <x:v>299</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>181</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1372,13 +1372,13 @@
         <x:v>154</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>108</x:v>
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>32</x:v>
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>98</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>131</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1580,13 +1580,13 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1606,13 +1606,13 @@
         <x:v>83</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1632,13 +1632,13 @@
         <x:v>167</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1658,13 +1658,13 @@
         <x:v>236</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>356</x:v>
+        <x:v>357</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>326</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>180</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1736,13 +1736,13 @@
         <x:v>107</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>279</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>281</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>394</x:v>
+        <x:v>397</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1866,13 +1866,13 @@
         <x:v>185</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1892,13 +1892,13 @@
         <x:v>263</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,16 +1967,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-23 18:01:09
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>83</x:v>
@@ -823,7 +823,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E8" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F8" s="0" t="n">
         <x:v>3</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>442</x:v>
+        <x:v>445</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>217</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>217</x:v>
+        <x:v>219</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>301</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>435</x:v>
+        <x:v>436</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>233</x:v>
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>57</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>91</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>77</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>110</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>299</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1372,13 +1372,13 @@
         <x:v>154</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>98</x:v>
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>38</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>236</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>107</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>357</x:v>
+        <x:v>361</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>327</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>282</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>282</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>397</x:v>
+        <x:v>400</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>87</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-23 23:00:47
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -693,16 +693,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>30</x:v>
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>445</x:v>
+        <x:v>448</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>219</x:v>
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>305</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>436</x:v>
+        <x:v>441</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>234</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>57</x:v>
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1086,13 +1086,13 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>28</x:v>
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>80</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>235</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>301</x:v>
+        <x:v>300</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>98</x:v>
@@ -1476,13 +1476,13 @@
         <x:v>260</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>197</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>38</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>69</x:v>
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>238</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>107</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>361</x:v>
+        <x:v>363</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>169</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>328</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>181</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>60</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>283</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>63</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>400</x:v>
+        <x:v>405</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>77</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>264</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>102</x:v>
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>11</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-24 07:00:52
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>83</x:v>
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>448</x:v>
+        <x:v>449</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>219</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>80</x:v>
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>64</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>79</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>329</x:v>
+        <x:v>331</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>284</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>154</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-24 12:00:57
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -748,13 +748,13 @@
         <x:v>128</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>449</x:v>
+        <x:v>452</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>228</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>312</x:v>
+        <x:v>313</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>441</x:v>
+        <x:v>444</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>234</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>234</x:v>
+        <x:v>245</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -956,13 +956,13 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -982,13 +982,13 @@
         <x:v>114</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1008,13 +1008,13 @@
         <x:v>145</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1060,13 +1060,13 @@
         <x:v>87</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1164,13 +1164,13 @@
         <x:v>131</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>184</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1242,13 +1242,13 @@
         <x:v>193</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>238</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1294,13 +1294,13 @@
         <x:v>143</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1320,13 +1320,13 @@
         <x:v>300</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>184</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>155</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>260</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1502,13 +1502,13 @@
         <x:v>199</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>132</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1580,13 +1580,13 @@
         <x:v>142</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>239</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>363</x:v>
+        <x:v>364</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>331</x:v>
+        <x:v>332</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1762,13 +1762,13 @@
         <x:v>291</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>285</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>405</x:v>
+        <x:v>409</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1866,13 +1866,13 @@
         <x:v>187</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>265</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1918,13 +1918,13 @@
         <x:v>228</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1944,13 +1944,13 @@
         <x:v>217</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-24 18:00:55
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>85</x:v>
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>452</x:v>
+        <x:v>456</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>228</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>313</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>175</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>444</x:v>
+        <x:v>451</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>245</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>245</x:v>
+        <x:v>246</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>82</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>105</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>242</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>300</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>67</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>88</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>113</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>262</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>136</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>72</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>79</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>364</x:v>
+        <x:v>370</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>172</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>332</x:v>
+        <x:v>338</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>183</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>291</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>286</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>409</x:v>
+        <x:v>415</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>201</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>78</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>267</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>115</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-24 23:00:51
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>61</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>456</x:v>
+        <x:v>468</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>315</x:v>
+        <x:v>317</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>175</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>451</x:v>
+        <x:v>456</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>63</x:v>
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>45</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>28</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>82</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>117</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>88</x:v>
@@ -1320,13 +1320,13 @@
         <x:v>305</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>88</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>113</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>265</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>136</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>199</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>85</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>72</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>54</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>240</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>111</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>370</x:v>
+        <x:v>374</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>172</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>338</x:v>
+        <x:v>342</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>295</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>288</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>159</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>415</x:v>
+        <x:v>419</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>201</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>78</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>105</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>217</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>90</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-25 07:01:00
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>26</x:v>
@@ -930,13 +930,13 @@
         <x:v>456</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -982,13 +982,13 @@
         <x:v>117</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1057,7 +1057,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>45</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>305</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>419</x:v>
+        <x:v>420</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>201</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-25 12:00:50
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -748,13 +748,13 @@
         <x:v>130</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>468</x:v>
+        <x:v>472</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>229</x:v>
+        <x:v>233</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -904,13 +904,13 @@
         <x:v>317</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>456</x:v>
+        <x:v>461</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>250</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>250</x:v>
+        <x:v>253</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -982,13 +982,13 @@
         <x:v>117</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>65</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>95</x:v>
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>25</x:v>
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1190,13 +1190,13 @@
         <x:v>158</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>247</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>306</x:v>
+        <x:v>307</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1372,13 +1372,13 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1398,13 +1398,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1424,13 +1424,13 @@
         <x:v>69</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1450,13 +1450,13 @@
         <x:v>173</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>268</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>85</x:v>
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1658,13 +1658,13 @@
         <x:v>243</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>374</x:v>
+        <x:v>377</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>342</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1762,13 +1762,13 @@
         <x:v>294</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>291</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1840,13 +1840,13 @@
         <x:v>420</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>205</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>230</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1944,13 +1944,13 @@
         <x:v>218</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-25 18:00:49
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -693,16 +693,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -722,13 +722,13 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>30</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>472</x:v>
+        <x:v>474</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>237</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>317</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>461</x:v>
+        <x:v>464</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>253</x:v>
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>63</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>65</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>95</x:v>
@@ -1060,13 +1060,13 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1083,16 +1083,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>190</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1268,13 +1268,13 @@
         <x:v>248</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1398,13 +1398,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,7 +1447,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
         <x:v>103</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>270</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>54</x:v>
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>243</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>377</x:v>
+        <x:v>378</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>344</x:v>
+        <x:v>349</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>294</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>147</x:v>
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>294</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>420</x:v>
+        <x:v>422</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>205</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>205</x:v>
+        <x:v>208</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>272</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>231</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>218</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-25 23:00:44
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>27</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>474</x:v>
+        <x:v>477</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>237</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>237</x:v>
+        <x:v>239</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>318</x:v>
+        <x:v>323</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>464</x:v>
+        <x:v>468</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>253</x:v>
+        <x:v>254</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>253</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>62</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>65</x:v>
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>85</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>199</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>248</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>309</x:v>
+        <x:v>310</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>151</x:v>
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>71</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>117</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>272</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>139</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>87</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>38</x:v>
@@ -1580,13 +1580,13 @@
         <x:v>149</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>54</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>82</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1684,13 +1684,13 @@
         <x:v>378</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>349</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>60</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>296</x:v>
+        <x:v>299</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>68</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>296</x:v>
+        <x:v>302</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>164</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>422</x:v>
+        <x:v>427</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>208</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>274</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>117</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>232</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-26 07:01:06
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>477</x:v>
+        <x:v>478</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>239</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>28</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>310</x:v>
+        <x:v>311</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>151</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>91</x:v>
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>31</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>273</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>87</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>352</x:v>
+        <x:v>354</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>190</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>427</x:v>
+        <x:v>428</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>208</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-26 12:00:50
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -670,13 +670,13 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -693,7 +693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>28</x:v>
@@ -748,13 +748,13 @@
         <x:v>130</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -774,13 +774,13 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>478</x:v>
+        <x:v>482</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>239</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>239</x:v>
+        <x:v>246</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>323</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>468</x:v>
+        <x:v>472</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>254</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>254</x:v>
+        <x:v>259</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -982,13 +982,13 @@
         <x:v>120</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1008,13 +1008,13 @@
         <x:v>155</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1034,13 +1034,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1135,16 +1135,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>191</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1242,13 +1242,13 @@
         <x:v>201</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>250</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1294,13 +1294,13 @@
         <x:v>150</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1320,13 +1320,13 @@
         <x:v>311</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>190</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1398,13 +1398,13 @@
         <x:v>196</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1450,13 +1450,13 @@
         <x:v>177</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>274</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>140</x:v>
@@ -1502,13 +1502,13 @@
         <x:v>207</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>143</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>73</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>54</x:v>
@@ -1632,13 +1632,13 @@
         <x:v>175</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1710,13 +1710,13 @@
         <x:v>354</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>60</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>299</x:v>
+        <x:v>300</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1814,13 +1814,13 @@
         <x:v>302</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>168</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>428</x:v>
+        <x:v>429</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>212</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1866,13 +1866,13 @@
         <x:v>192</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1892,13 +1892,13 @@
         <x:v>276</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>234</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1944,13 +1944,13 @@
         <x:v>221</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-26 18:00:58
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>89</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>482</x:v>
+        <x:v>490</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>248</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>324</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>472</x:v>
+        <x:v>478</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>259</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>259</x:v>
+        <x:v>261</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>155</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>96</x:v>
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>110</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>311</x:v>
+        <x:v>313</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>154</x:v>
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>92</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1421,16 +1421,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>276</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1502,13 +1502,13 @@
         <x:v>207</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>38</x:v>
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>250</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>354</x:v>
+        <x:v>358</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>68</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>429</x:v>
+        <x:v>430</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>85</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>235</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>109</x:v>
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,16 +1967,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-26 23:00:43
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -719,7 +719,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>27</x:v>
@@ -745,16 +745,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>490</x:v>
+        <x:v>502</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>248</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>248</x:v>
+        <x:v>250</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>325</x:v>
+        <x:v>332</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>185</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>478</x:v>
+        <x:v>492</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>64</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>86</x:v>
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>110</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>251</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>124</x:v>
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>279</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>142</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>207</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>89</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>73</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>378</x:v>
+        <x:v>380</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>175</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>358</x:v>
+        <x:v>364</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>61</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>300</x:v>
+        <x:v>303</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>68</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>430</x:v>
+        <x:v>435</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>85</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>276</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>119</x:v>
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>234</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>109</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>225</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>97</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-27 07:01:03
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>502</x:v>
+        <x:v>503</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>250</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>92</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>144</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>435</x:v>
+        <x:v>436</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>85</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>224</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>97</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-27 12:00:48
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>503</x:v>
+        <x:v>506</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>250</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>250</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>332</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>492</x:v>
+        <x:v>494</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>262</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>262</x:v>
+        <x:v>269</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -956,13 +956,13 @@
         <x:v>124</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1008,13 +1008,13 @@
         <x:v>159</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1034,13 +1034,13 @@
         <x:v>196</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1060,13 +1060,13 @@
         <x:v>95</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1138,13 +1138,13 @@
         <x:v>84</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1190,13 +1190,13 @@
         <x:v>162</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1242,13 +1242,13 @@
         <x:v>206</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1294,13 +1294,13 @@
         <x:v>152</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>313</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>191</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1372,13 +1372,13 @@
         <x:v>164</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>281</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1580,13 +1580,13 @@
         <x:v>151</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1606,13 +1606,13 @@
         <x:v>88</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1629,16 +1629,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>252</x:v>
+        <x:v>254</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>120</x:v>
@@ -1684,13 +1684,13 @@
         <x:v>380</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>175</x:v>
+        <x:v>177</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>364</x:v>
+        <x:v>367</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>203</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>302</x:v>
+        <x:v>303</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>168</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>436</x:v>
+        <x:v>438</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>216</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>216</x:v>
+        <x:v>221</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>277</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>235</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1944,13 +1944,13 @@
         <x:v>225</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-27 16:23:46
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -673,10 +673,10 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -699,10 +699,10 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -725,10 +725,10 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -751,10 +751,10 @@
         <x:v>90</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -777,10 +777,10 @@
         <x:v>31</x:v>
       </x:c>
       <x:c r="G6" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -803,10 +803,10 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="G7" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
@@ -829,10 +829,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="G8" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H8" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>506</x:v>
+        <x:v>510</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>255</x:v>
+        <x:v>351</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -907,10 +907,10 @@
         <x:v>186</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>494</x:v>
+        <x:v>499</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>356</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>68</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -985,10 +985,10 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1011,10 +1011,10 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1037,10 +1037,10 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>53</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1089,10 +1089,10 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="G18" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
@@ -1115,10 +1115,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G19" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H19" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:8">
@@ -1135,16 +1135,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>30</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1161,16 +1161,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>74</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1219,10 +1219,10 @@
         <x:v>92</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1245,10 +1245,10 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>125</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1297,10 +1297,10 @@
         <x:v>94</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>315</x:v>
+        <x:v>317</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>239</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1349,10 +1349,10 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>119</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>171</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1427,10 +1427,10 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="G31" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8">
@@ -1453,10 +1453,10 @@
         <x:v>106</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>282</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>233</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>210</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>139</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>90</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>74</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,16 +1603,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>55</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1635,10 +1635,10 @@
         <x:v>88</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>254</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>120</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>200</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1687,10 +1687,10 @@
         <x:v>177</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>269</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>367</x:v>
+        <x:v>370</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>264</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>61</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>303</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>154</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>222</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>70</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>303</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>168</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>231</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>438</x:v>
+        <x:v>440</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>221</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>313</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1869,10 +1869,10 @@
         <x:v>87</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>279</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>120</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>207</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1921,10 +1921,10 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>225</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>98</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1973,10 +1973,10 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="G52" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="H52" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-27 18:00:56
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>64</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>510</x:v>
+        <x:v>513</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>256</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>95</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>351</x:v>
+        <x:v>353</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>333</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>186</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>254</x:v>
+        <x:v>253</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>499</x:v>
+        <x:v>501</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>273</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>356</x:v>
+        <x:v>357</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -956,13 +956,13 @@
         <x:v>126</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>34</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>197</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>51</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1320,13 +1320,13 @@
         <x:v>317</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>81</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>239</x:v>
+        <x:v>240</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>74</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>199</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>52</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>283</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>144</x:v>
@@ -1502,13 +1502,13 @@
         <x:v>211</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>39</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1528,13 +1528,13 @@
         <x:v>145</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>27</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>39</x:v>
@@ -1658,13 +1658,13 @@
         <x:v>255</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>80</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>200</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1840,13 +1840,13 @@
         <x:v>440</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>313</x:v>
+        <x:v>314</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>236</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>73</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-27 23:00:50
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>64</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>513</x:v>
+        <x:v>518</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>258</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>353</x:v>
+        <x:v>351</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>334</x:v>
+        <x:v>337</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>186</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>253</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>501</x:v>
+        <x:v>506</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>273</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>84</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>357</x:v>
+        <x:v>360</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -979,7 +979,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
         <x:v>66</x:v>
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>70</x:v>
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>196</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>100</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>74</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>93</x:v>
@@ -1239,16 +1239,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="G24" s="0" t="n">
         <x:v>30</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8">
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>60</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>317</x:v>
+        <x:v>320</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>81</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>240</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>52</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>200</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>120</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>284</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>89</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>234</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>74</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>370</x:v>
+        <x:v>372</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>204</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>60</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>264</x:v>
+        <x:v>265</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>305</x:v>
+        <x:v>309</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>154</x:v>
@@ -1785,16 +1785,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>39</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>306</x:v>
+        <x:v>311</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>63</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>231</x:v>
+        <x:v>232</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>440</x:v>
+        <x:v>443</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>222</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>314</x:v>
+        <x:v>315</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>199</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>44</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>280</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>120</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>237</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>73</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>226</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>72</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>170</x:v>
+        <x:v>171</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>12</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-28 07:01:02
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>518</x:v>
+        <x:v>520</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>257</x:v>
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>337</x:v>
+        <x:v>336</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>186</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>254</x:v>
+        <x:v>253</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>506</x:v>
+        <x:v>509</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>276</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>360</x:v>
+        <x:v>361</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>69</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>120</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>281</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>120</x:v>
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>99</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-28 12:00:47
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>520</x:v>
+        <x:v>522</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>257</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>336</x:v>
+        <x:v>339</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>186</x:v>
@@ -927,7 +927,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>509</x:v>
+        <x:v>513</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
         <x:v>276</x:v>
@@ -982,13 +982,13 @@
         <x:v>125</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>35</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>49</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>32</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>287</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>145</x:v>
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>140</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>74</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>121</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>380</x:v>
+        <x:v>381</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>177</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>372</x:v>
+        <x:v>374</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>205</x:v>
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>61</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>69</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>443</x:v>
+        <x:v>445</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>315</x:v>
+        <x:v>316</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>88</x:v>
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>282</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>120</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>238</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>73</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1944,13 +1944,13 @@
         <x:v>228</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>72</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-28 18:00:55
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>522</x:v>
+        <x:v>527</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>257</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>339</x:v>
+        <x:v>341</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>186</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>513</x:v>
+        <x:v>518</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>276</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>85</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>361</x:v>
+        <x:v>364</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>69</x:v>
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>49</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>48</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1057,16 +1057,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>24</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>113</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>320</x:v>
+        <x:v>321</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>81</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>241</x:v>
+        <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>41</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>120</x:v>
@@ -1421,7 +1421,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F31" s="0" t="n">
         <x:v>32</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1499,7 +1499,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
         <x:v>140</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>155</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>74</x:v>
@@ -1788,13 +1788,13 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>39</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>311</x:v>
+        <x:v>314</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>169</x:v>
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>445</x:v>
+        <x:v>447</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>224</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>88</x:v>
@@ -1892,13 +1892,13 @@
         <x:v>283</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>87</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>207</x:v>
+        <x:v>208</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-28 23:00:51
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>527</x:v>
+        <x:v>529</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>94</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>351</x:v>
+        <x:v>352</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>341</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>186</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>518</x:v>
+        <x:v>520</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>279</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>85</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>364</x:v>
+        <x:v>365</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>34</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -982,10 +982,10 @@
         <x:v>125</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
         <x:v>100</x:v>
@@ -1008,10 +1008,10 @@
         <x:v>163</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
         <x:v>121</x:v>
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>88</x:v>
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>94</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>321</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>161</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>120</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>288</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>89</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>234</x:v>
+        <x:v>235</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>91</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>39</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>55</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>88</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>121</x:v>
@@ -1710,13 +1710,13 @@
         <x:v>374</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>205</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>60</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>265</x:v>
+        <x:v>266</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>61</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>70</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>314</x:v>
+        <x:v>316</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>63</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>232</x:v>
+        <x:v>234</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>204</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>44</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1889,7 +1889,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>283</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
         <x:v>121</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>239</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>114</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>228</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-29 07:01:00
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,7 +875,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>529</x:v>
+        <x:v>531</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
         <x:v>258</x:v>
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>344</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>186</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-29 12:00:45
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -693,7 +693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>28</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>531</x:v>
+        <x:v>536</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>258</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>94</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>352</x:v>
+        <x:v>353</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>343</x:v>
+        <x:v>347</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>186</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>520</x:v>
+        <x:v>521</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>280</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>85</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>365</x:v>
+        <x:v>366</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>71</x:v>
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>48</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1083,7 +1083,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>26</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>74</x:v>
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>165</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>42</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>322</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>81</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>242</x:v>
+        <x:v>243</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>93</x:v>
@@ -1577,7 +1577,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
         <x:v>74</x:v>
@@ -1629,7 +1629,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
         <x:v>88</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>381</x:v>
+        <x:v>382</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>271</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>374</x:v>
+        <x:v>375</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>60</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>266</x:v>
+        <x:v>267</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>28</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-29 18:00:53
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -745,7 +745,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
         <x:v>90</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>536</x:v>
+        <x:v>545</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>259</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>353</x:v>
+        <x:v>356</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,13 +901,13 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>347</x:v>
+        <x:v>350</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
         <x:v>253</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>521</x:v>
+        <x:v>528</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>281</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>85</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>366</x:v>
+        <x:v>369</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>34</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -1005,7 +1005,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
         <x:v>71</x:v>
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>93</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>258</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>60</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>94</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>324</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>162</x:v>
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>75</x:v>
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>204</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>120</x:v>
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>291</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>146</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>39</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>91</x:v>
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>55</x:v>
@@ -1655,16 +1655,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>257</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>80</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>382</x:v>
+        <x:v>384</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>179</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>375</x:v>
+        <x:v>376</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>207</x:v>
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
         <x:v>28</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>70</x:v>
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>316</x:v>
+        <x:v>320</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>63</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>234</x:v>
+        <x:v>236</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,7 +1837,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>447</x:v>
+        <x:v>450</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
         <x:v>224</x:v>
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>206</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>89</x:v>
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>237</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
         <x:v>72</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>186</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>230</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>101</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-29 23:00:47
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,7 +667,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>66</x:v>
@@ -693,7 +693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>28</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>545</x:v>
+        <x:v>552</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>95</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>356</x:v>
+        <x:v>357</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>350</x:v>
+        <x:v>354</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>253</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>528</x:v>
+        <x:v>544</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>284</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>369</x:v>
+        <x:v>371</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>48</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1187,7 +1187,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
         <x:v>89</x:v>
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>209</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>113</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>261</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>60</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,16 +1291,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G26" s="0" t="n">
         <x:v>25</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8">
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>325</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>162</x:v>
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>194</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>75</x:v>
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>41</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>205</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>52</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,7 +1473,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>292</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>146</x:v>
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>39</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>27</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>157</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>37</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>384</x:v>
+        <x:v>387</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>179</x:v>
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>376</x:v>
+        <x:v>379</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>207</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>267</x:v>
+        <x:v>269</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,16 +1733,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>63</x:v>
       </x:c>
       <x:c r="G43" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H43" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:8">
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>309</x:v>
+        <x:v>311</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>154</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>320</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>173</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>450</x:v>
+        <x:v>453</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>224</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>316</x:v>
+        <x:v>317</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>44</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1941,7 +1941,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>232</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
         <x:v>101</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-30 07:00:54
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>552</x:v>
+        <x:v>555</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>262</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>95</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>357</x:v>
+        <x:v>359</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>354</x:v>
+        <x:v>355</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>65</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>254</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -979,16 +979,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>34</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>50</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>199</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>51</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1343,7 +1343,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
         <x:v>75</x:v>
@@ -1528,13 +1528,13 @@
         <x:v>149</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>27</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>387</x:v>
+        <x:v>388</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>179</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-30 12:00:53
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -667,16 +667,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -748,13 +748,13 @@
         <x:v>135</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G5" s="0" t="n">
         <x:v>11</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>555</x:v>
+        <x:v>559</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>264</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>95</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>359</x:v>
+        <x:v>371</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>355</x:v>
+        <x:v>358</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
-        <x:v>190</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
         <x:v>65</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>255</x:v>
+        <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>544</x:v>
+        <x:v>547</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>285</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>86</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>371</x:v>
+        <x:v>380</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,16 +953,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G13" s="0" t="n">
         <x:v>34</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8">
@@ -982,13 +982,13 @@
         <x:v>124</x:v>
       </x:c>
       <x:c r="F14" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G14" s="0" t="n">
         <x:v>34</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8">
@@ -1060,13 +1060,13 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="G17" s="0" t="n">
         <x:v>24</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8">
@@ -1138,13 +1138,13 @@
         <x:v>86</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G20" s="0" t="n">
         <x:v>37</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8">
@@ -1164,13 +1164,13 @@
         <x:v>138</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G21" s="0" t="n">
         <x:v>31</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8">
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>42</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,16 +1213,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>200</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>51</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1268,13 +1268,13 @@
         <x:v>266</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>60</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>328</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>162</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>81</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>243</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1346,13 +1346,13 @@
         <x:v>198</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>52</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>127</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1369,7 +1369,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
         <x:v>94</x:v>
@@ -1395,16 +1395,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="G30" s="0" t="n">
         <x:v>52</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8">
@@ -1476,13 +1476,13 @@
         <x:v>293</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>89</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>235</x:v>
+        <x:v>239</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>216</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>142</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>39</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>181</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>27</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1554,13 +1554,13 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>37</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1606,13 +1606,13 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G38" s="0" t="n">
         <x:v>16</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8">
@@ -1632,13 +1632,13 @@
         <x:v>180</x:v>
       </x:c>
       <x:c r="F39" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G39" s="0" t="n">
         <x:v>51</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8">
@@ -1658,13 +1658,13 @@
         <x:v>259</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="G40" s="0" t="n">
         <x:v>80</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>202</x:v>
+        <x:v>204</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8">
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>388</x:v>
+        <x:v>389</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>271</x:v>
+        <x:v>277</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>379</x:v>
+        <x:v>380</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>61</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>275</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1733,7 +1733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="F43" s="0" t="n">
         <x:v>63</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>311</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>154</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>68</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>222</x:v>
+        <x:v>226</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1788,13 +1788,13 @@
         <x:v>144</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G45" s="0" t="n">
         <x:v>39</x:v>
       </x:c>
       <x:c r="H45" s="0" t="n">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>322</x:v>
+        <x:v>323</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>63</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>236</x:v>
+        <x:v>240</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1840,13 +1840,13 @@
         <x:v>453</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>225</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>317</x:v>
+        <x:v>323</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,16 +1863,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>44</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1892,13 +1892,13 @@
         <x:v>284</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>87</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>208</x:v>
+        <x:v>211</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1944,13 +1944,13 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>73</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>174</x:v>
+        <x:v>177</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>12</x:v>

</xml_diff>

<commit_message>
Commit via gitrun.py em 2024-09-30 18:00:53
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -693,16 +693,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G3" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -719,16 +719,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -771,7 +771,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>31</x:v>
@@ -823,7 +823,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E8" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F8" s="0" t="n">
         <x:v>3</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>559</x:v>
+        <x:v>568</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>276</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>371</x:v>
+        <x:v>376</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,16 +901,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>358</x:v>
+        <x:v>361</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>195</x:v>
       </x:c>
       <x:c r="G11" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>260</x:v>
+        <x:v>259</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>547</x:v>
+        <x:v>552</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>294</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>86</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>380</x:v>
+        <x:v>381</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -953,7 +953,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F13" s="0" t="n">
         <x:v>74</x:v>
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>50</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,16 +1031,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="G16" s="0" t="n">
         <x:v>48</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -1109,7 +1109,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E19" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F19" s="0" t="n">
         <x:v>5</x:v>
@@ -1135,7 +1135,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F20" s="0" t="n">
         <x:v>31</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>75</x:v>
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>42</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1213,7 +1213,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
-        <x:v>201</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
         <x:v>95</x:v>
@@ -1265,7 +1265,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>266</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
         <x:v>131</x:v>
@@ -1317,16 +1317,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>329</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="G27" s="0" t="n">
         <x:v>81</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>251</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8">
@@ -1343,16 +1343,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>198</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F28" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="G28" s="0" t="n">
         <x:v>52</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8">
@@ -1372,13 +1372,13 @@
         <x:v>169</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>41</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1447,16 +1447,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
-        <x:v>182</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F32" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="G32" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>293</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>89</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>239</x:v>
+        <x:v>240</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1499,16 +1499,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>217</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="F34" s="0" t="n">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G34" s="0" t="n">
         <x:v>39</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8">
@@ -1525,16 +1525,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G35" s="0" t="n">
         <x:v>27</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8">
@@ -1551,16 +1551,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G36" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8">
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>161</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>37</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>259</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>124</x:v>
@@ -1681,16 +1681,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>389</x:v>
+        <x:v>393</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>277</x:v>
+        <x:v>278</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1707,16 +1707,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>380</x:v>
+        <x:v>383</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
-        <x:v>214</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="G42" s="0" t="n">
         <x:v>61</x:v>
       </x:c>
       <x:c r="H42" s="0" t="n">
-        <x:v>275</x:v>
+        <x:v>276</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:8">
@@ -1759,7 +1759,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>312</x:v>
+        <x:v>313</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
         <x:v>158</x:v>
@@ -1785,7 +1785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
-        <x:v>144</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="F45" s="0" t="n">
         <x:v>72</x:v>
@@ -1811,7 +1811,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>323</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
         <x:v>177</x:v>
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>453</x:v>
+        <x:v>460</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>231</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>323</x:v>
+        <x:v>326</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1863,7 +1863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
         <x:v>94</x:v>
@@ -1889,16 +1889,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>284</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>87</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>213</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -1915,7 +1915,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>241</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>116</x:v>
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>233</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>104</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
         <x:v>73</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>12</x:v>

</xml_diff>

<commit_message>
Data update using git
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_Integrado.xlsx
@@ -670,13 +670,13 @@
         <x:v>98</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G2" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -797,7 +797,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
         <x:v>16</x:v>
@@ -875,16 +875,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>568</x:v>
+        <x:v>576</x:v>
       </x:c>
       <x:c r="F10" s="0" t="n">
-        <x:v>280</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="G10" s="0" t="n">
         <x:v>96</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>376</x:v>
+        <x:v>380</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
@@ -901,7 +901,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
-        <x:v>361</x:v>
+        <x:v>362</x:v>
       </x:c>
       <x:c r="F11" s="0" t="n">
         <x:v>195</x:v>
@@ -927,16 +927,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
-        <x:v>552</x:v>
+        <x:v>561</x:v>
       </x:c>
       <x:c r="F12" s="0" t="n">
-        <x:v>295</x:v>
+        <x:v>299</x:v>
       </x:c>
       <x:c r="G12" s="0" t="n">
         <x:v>86</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>381</x:v>
+        <x:v>385</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8">
@@ -1005,16 +1005,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>168</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>50</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1031,7 +1031,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
-        <x:v>204</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F16" s="0" t="n">
         <x:v>104</x:v>
@@ -1161,7 +1161,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F21" s="0" t="n">
         <x:v>75</x:v>
@@ -1187,16 +1187,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F22" s="0" t="n">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G22" s="0" t="n">
         <x:v>42</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8">
@@ -1216,13 +1216,13 @@
         <x:v>203</x:v>
       </x:c>
       <x:c r="F23" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G23" s="0" t="n">
         <x:v>51</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8">
@@ -1239,7 +1239,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
-        <x:v>210</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="F24" s="0" t="n">
         <x:v>113</x:v>
@@ -1265,16 +1265,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
-        <x:v>269</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="F25" s="0" t="n">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="G25" s="0" t="n">
         <x:v>60</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8">
@@ -1291,7 +1291,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
-        <x:v>156</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F26" s="0" t="n">
         <x:v>95</x:v>
@@ -1317,7 +1317,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>333</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="F27" s="0" t="n">
         <x:v>170</x:v>
@@ -1369,16 +1369,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="F29" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G29" s="0" t="n">
         <x:v>41</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8">
@@ -1395,7 +1395,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>211</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="F30" s="0" t="n">
         <x:v>126</x:v>
@@ -1473,16 +1473,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>294</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="G33" s="0" t="n">
         <x:v>89</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>240</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8">
@@ -1525,7 +1525,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F35" s="0" t="n">
         <x:v>97</x:v>
@@ -1551,7 +1551,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F36" s="0" t="n">
         <x:v>43</x:v>
@@ -1577,16 +1577,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F37" s="0" t="n">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G37" s="0" t="n">
         <x:v>37</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8">
@@ -1603,7 +1603,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F38" s="0" t="n">
         <x:v>58</x:v>
@@ -1655,7 +1655,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
-        <x:v>262</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="F40" s="0" t="n">
         <x:v>124</x:v>
@@ -1681,7 +1681,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>393</x:v>
+        <x:v>394</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
         <x:v>186</x:v>
@@ -1707,7 +1707,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
-        <x:v>383</x:v>
+        <x:v>385</x:v>
       </x:c>
       <x:c r="F42" s="0" t="n">
         <x:v>215</x:v>
@@ -1759,16 +1759,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
-        <x:v>313</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="F44" s="0" t="n">
-        <x:v>158</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="G44" s="0" t="n">
         <x:v>68</x:v>
       </x:c>
       <x:c r="H44" s="0" t="n">
-        <x:v>226</x:v>
+        <x:v>225</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:8">
@@ -1811,16 +1811,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>325</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>63</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>240</x:v>
+        <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1837,16 +1837,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>460</x:v>
+        <x:v>461</x:v>
       </x:c>
       <x:c r="F47" s="0" t="n">
-        <x:v>234</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="G47" s="0" t="n">
         <x:v>92</x:v>
       </x:c>
       <x:c r="H47" s="0" t="n">
-        <x:v>326</x:v>
+        <x:v>327</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:8">
@@ -1915,16 +1915,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="F50" s="0" t="n">
         <x:v>116</x:v>
       </x:c>
       <x:c r="G50" s="0" t="n">
-        <x:v>72</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="H50" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:8">
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>238</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="F51" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G51" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="H51" s="0" t="n">
-        <x:v>179</x:v>
+        <x:v>181</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:8">
@@ -1967,7 +1967,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F52" s="0" t="n">
         <x:v>12</x:v>

</xml_diff>